<commit_message>
change of respository create new file to merged_data insertion data upload sql code finally homewrok
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\Semestre 6\Bases de datos II\Python_db_2024_02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350F128D-36A8-4F97-85FF-D3E4F3CC2DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECABD49-D614-400E-AAF1-706F940F3D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>OrderID</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>Avenida 4 #56-78, Manizales</t>
-  </si>
-  <si>
-    <t>total_price</t>
   </si>
 </sst>
 </file>
@@ -546,10 +543,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,7 +557,7 @@
     <col min="5" max="6" width="14" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -579,11 +576,8 @@
       <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>3001</v>
       </c>
@@ -603,7 +597,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>3002</v>
       </c>
@@ -623,7 +617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3003</v>
       </c>
@@ -643,7 +637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3004</v>
       </c>
@@ -663,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3005</v>
       </c>
@@ -683,7 +677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>3006</v>
       </c>
@@ -703,7 +697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>3007</v>
       </c>
@@ -723,7 +717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>3008</v>
       </c>
@@ -743,7 +737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>3009</v>
       </c>
@@ -763,7 +757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>3010</v>
       </c>
@@ -783,7 +777,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>3011</v>
       </c>
@@ -803,7 +797,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>3012</v>
       </c>
@@ -823,7 +817,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>3013</v>
       </c>
@@ -843,7 +837,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>3014</v>
       </c>
@@ -863,7 +857,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>3015</v>
       </c>

</xml_diff>